<commit_message>
CO2-Test ok (o poti)
</commit_message>
<xml_diff>
--- a/esp32-test_conn.xlsx
+++ b/esp32-test_conn.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>OLED</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>I2C2</t>
+  </si>
+  <si>
+    <t>MQ135 Gas</t>
+  </si>
+  <si>
+    <t>int LED nio</t>
   </si>
 </sst>
 </file>
@@ -78,12 +84,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,11 +122,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -125,32 +152,69 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>63868</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>716050</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9470</xdr:rowOff>
+      <xdr:colOff>707095</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>101601</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Grafik 13"/>
+        <xdr:cNvPr id="17" name="Grafik 16"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="24313" r="25576"/>
+        <a:srcRect l="24824" r="24776"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5473700" y="406399"/>
-          <a:ext cx="4449850" cy="4746571"/>
+          <a:off x="5423268" y="431800"/>
+          <a:ext cx="4453227" cy="4622801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2298700</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>115157</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Grafik 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="75153"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="127000" y="495300"/>
+          <a:ext cx="2171700" cy="4572857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -162,32 +226,32 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>2209800</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9470</xdr:rowOff>
+      <xdr:colOff>2199786</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>89757</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Grafik 14"/>
+        <xdr:cNvPr id="19" name="Grafik 18"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="74369" r="1032"/>
+        <a:srcRect l="75413"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13804900" y="406399"/>
-          <a:ext cx="2184400" cy="4746571"/>
+          <a:off x="13792200" y="469900"/>
+          <a:ext cx="2148986" cy="4572857"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -198,33 +262,34 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2273300</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9470</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>68416</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Grafik 15"/>
+        <xdr:cNvPr id="20" name="Grafik 19"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="-429" r="75687"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76200" y="406399"/>
-          <a:ext cx="2197100" cy="4746571"/>
+          <a:off x="4597400" y="5156200"/>
+          <a:ext cx="6164416" cy="3759200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -502,7 +567,7 @@
   <dimension ref="B7:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +594,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L9" t="s">
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -537,19 +605,22 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
+      <c r="L10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L12" t="s">
+      <c r="L12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -562,24 +633,22 @@
       </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="M22" t="s">
+      <c r="M22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="E24" s="1" t="s">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="P26" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="P26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Testing with CO2 measure ok
</commit_message>
<xml_diff>
--- a/esp32-test_conn.xlsx
+++ b/esp32-test_conn.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="18855" windowHeight="12510"/>
+    <workbookView xWindow="3330" yWindow="0" windowWidth="18855" windowHeight="12510"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="ESP32_NodeMCU" sheetId="1" r:id="rId1"/>
+    <sheet name="ESP32_D1" sheetId="2" r:id="rId2"/>
+    <sheet name="RTC_D1_Shield" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>OLED</t>
   </si>
@@ -32,24 +34,6 @@
     <t>debug lila</t>
   </si>
   <si>
-    <t>debug oran</t>
-  </si>
-  <si>
-    <t>debug  grün</t>
-  </si>
-  <si>
-    <t>debug blau</t>
-  </si>
-  <si>
-    <t>debug gelb</t>
-  </si>
-  <si>
-    <t>debug schw</t>
-  </si>
-  <si>
-    <t>debug rot</t>
-  </si>
-  <si>
     <t>5 V</t>
   </si>
   <si>
@@ -69,6 +53,108 @@
   </si>
   <si>
     <t>int LED nio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QM135Gas </t>
+  </si>
+  <si>
+    <t>Ampel rt</t>
+  </si>
+  <si>
+    <t>I2C2 SCL</t>
+  </si>
+  <si>
+    <t>Ampel ge</t>
+  </si>
+  <si>
+    <t>I2C2 SDA</t>
+  </si>
+  <si>
+    <t>Ampel gr</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>SD CS</t>
+  </si>
+  <si>
+    <t>SD MOSI</t>
+  </si>
+  <si>
+    <t>SD MISO</t>
+  </si>
+  <si>
+    <t>SD SCK</t>
+  </si>
+  <si>
+    <t>FRAM</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>BME 280</t>
+  </si>
+  <si>
+    <t>Die Anschluesse muessen auf der LP</t>
+  </si>
+  <si>
+    <t>verfolgt und ev getrennt/verbundenwerden</t>
+  </si>
+  <si>
+    <t>RTC SDA</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>RTC SCL</t>
+  </si>
+  <si>
+    <t>SCK</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>RTC_SCA</t>
+  </si>
+  <si>
+    <t>Ana Vorabe</t>
+  </si>
+  <si>
+    <t>debug red</t>
+  </si>
+  <si>
+    <t>debug blue</t>
+  </si>
+  <si>
+    <t>debug yellow</t>
+  </si>
+  <si>
+    <t>debug orange</t>
+  </si>
+  <si>
+    <t>debug  green</t>
+  </si>
+  <si>
+    <t>debug black</t>
+  </si>
+  <si>
+    <t>Gas Ajust</t>
   </si>
 </sst>
 </file>
@@ -290,6 +376,332 @@
         <a:xfrm>
           <a:off x="4597400" y="5156200"/>
           <a:ext cx="6164416" cy="3759200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>115456</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>109038</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6588044" cy="5750280"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="21160" r="21182"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6973456" y="1061538"/>
+          <a:ext cx="6588044" cy="5750280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>57736</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>115456</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2389682" cy="5749333"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="79082"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17583736" y="1067956"/>
+          <a:ext cx="2389682" cy="5749333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>634991</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43298</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2392186" cy="5749333"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="79060"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1396991" y="995798"/>
+          <a:ext cx="2392186" cy="5749333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8874666" cy="1237333"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6944591" y="7048499"/>
+          <a:ext cx="8874666" cy="1237333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>115456</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>51310</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>582309</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>158751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="21160" r="21182"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6973456" y="1003810"/>
+          <a:ext cx="6553328" cy="5822441"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>57736</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43296</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>152759</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>164220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="79082"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16726486" y="995796"/>
+          <a:ext cx="2381023" cy="5835924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>634991</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>43298</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>732518</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>164222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="79060"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1396991" y="995798"/>
+          <a:ext cx="2383527" cy="5835924"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>86591</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>-1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>648529</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>111651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6944591" y="7048499"/>
+          <a:ext cx="8848688" cy="1254652"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>145369</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>101022</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>643317</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>153073</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7221555" y="1997386"/>
+          <a:ext cx="6148051" cy="3879323"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -566,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,10 +991,10 @@
   <sheetData>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
@@ -590,12 +1002,12 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>0</v>
@@ -603,10 +1015,13 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
       </c>
       <c r="L10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -616,35 +1031,35 @@
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="L20" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="M22" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
@@ -655,4 +1070,218 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="H16:W33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="19" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="W16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="W20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="W21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="W23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="T24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="T25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="T28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="U29" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>15</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="H32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="F6:T17"/>
+  <sheetViews>
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="19" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
base ok - try toimplement ESP async webserver
</commit_message>
<xml_diff>
--- a/esp32-test_conn.xlsx
+++ b/esp32-test_conn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="0" windowWidth="18855" windowHeight="12510"/>
+    <workbookView xWindow="4440" yWindow="0" windowWidth="18855" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32_NodeMCU" sheetId="1" r:id="rId1"/>
@@ -139,22 +139,22 @@
     <t>debug red</t>
   </si>
   <si>
-    <t>debug blue</t>
-  </si>
-  <si>
-    <t>debug yellow</t>
-  </si>
-  <si>
-    <t>debug orange</t>
-  </si>
-  <si>
-    <t>debug  green</t>
-  </si>
-  <si>
-    <t>debug black</t>
-  </si>
-  <si>
     <t>Gas Ajust</t>
+  </si>
+  <si>
+    <t>debug yellow (TMS)</t>
+  </si>
+  <si>
+    <t>debug  green (TDI)</t>
+  </si>
+  <si>
+    <t>debug black (GND)</t>
+  </si>
+  <si>
+    <t>debug orange (TCK)</t>
+  </si>
+  <si>
+    <t>(TDO) debug blue</t>
   </si>
 </sst>
 </file>
@@ -208,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -216,6 +216,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -978,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,12 +1039,12 @@
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" t="s">
         <v>4</v>
@@ -1049,12 +1052,12 @@
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="M22" s="2" t="s">
-        <v>37</v>
+      <c r="M22" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
@@ -1171,7 +1174,7 @@
     </row>
     <row r="32" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H32" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
thermo couple type K included
</commit_message>
<xml_diff>
--- a/esp32-test_conn.xlsx
+++ b/esp32-test_conn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="0" windowWidth="18855" windowHeight="12510"/>
+    <workbookView xWindow="5550" yWindow="0" windowWidth="18855" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32_NodeMCU" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>RTC_SCA</t>
   </si>
   <si>
-    <t>Ana Vorabe</t>
-  </si>
-  <si>
     <t>debug red</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>(TDO) debug blue</t>
+  </si>
+  <si>
+    <t>Ana Vorgabe</t>
   </si>
 </sst>
 </file>
@@ -982,7 +982,7 @@
   <dimension ref="B7:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +994,7 @@
   <sheetData>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L7" t="s">
         <v>3</v>
@@ -1021,7 +1021,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="L10" t="s">
         <v>8</v>
@@ -1034,17 +1034,17 @@
     </row>
     <row r="18" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L20" t="s">
         <v>4</v>
@@ -1052,12 +1052,12 @@
     </row>
     <row r="21" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="4:16" x14ac:dyDescent="0.25">
       <c r="M22" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="4:16" x14ac:dyDescent="0.25">
@@ -1174,7 +1174,7 @@
     </row>
     <row r="32" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U32" s="2" t="s">
         <v>12</v>

</xml_diff>